<commit_message>
updated sample excel file
</commit_message>
<xml_diff>
--- a/src/test/data/all_data/bioproject_test_merge_cells.xlsx
+++ b/src/test/data/all_data/bioproject_test_merge_cells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoko/DDBJ/ddbj_validator/src/test/data/all_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B3D3D8-1B30-B945-B7C3-5D219F8EF2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49E6A5A-801D-E34E-AE4C-99E25E379B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6220" yWindow="5340" windowWidth="27500" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -594,9 +594,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.0000"/>
+    <numFmt numFmtId="176" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -642,6 +642,24 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -698,7 +716,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -737,10 +755,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -1975,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -2242,7 +2263,7 @@
       <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="20" t="s">
         <v>151</v>
       </c>
       <c r="C16" s="7"/>
@@ -2369,7 +2390,7 @@
       <c r="B23" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="22" t="s">
         <v>161</v>
       </c>
       <c r="D23" s="7"/>
@@ -2437,7 +2458,9 @@
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="7"/>
+      <c r="B27" s="11">
+        <v>12.3</v>
+      </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -2452,7 +2475,9 @@
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="11">
+        <v>12.3</v>
+      </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -2470,7 +2495,7 @@
       <c r="B29" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="21" t="s">
         <v>158</v>
       </c>
       <c r="D29" s="7"/>

</xml_diff>